<commit_message>
[GEN Main] issue 및 Sch update
</commit_message>
<xml_diff>
--- a/Plasma LF Issue List V1.0.xlsx
+++ b/Plasma LF Issue List V1.0.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Femto work" sheetId="5" r:id="rId1"/>
     <sheet name="GEN MCU" sheetId="1" r:id="rId2"/>
-    <sheet name="GEN" sheetId="2" r:id="rId3"/>
+    <sheet name="GEN Main" sheetId="2" r:id="rId3"/>
     <sheet name="Ctrl MCU" sheetId="4" r:id="rId4"/>
-    <sheet name="Ctrl PCB" sheetId="3" r:id="rId5"/>
+    <sheet name="Ctrl Main" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,18 +44,6 @@
     <t>Board dead 원인 파악</t>
   </si>
   <si>
-    <t>DC-DC Regulator가 dead 되는지 확인</t>
-  </si>
-  <si>
-    <t>FST10-5FFM</t>
-  </si>
-  <si>
-    <t>Fuse dead 발생 여부</t>
-  </si>
-  <si>
-    <t>250VAC 5A</t>
-  </si>
-  <si>
     <t>Transformer 1,2차 coil중 어느쪽이 dead되는지 확인 - 1차측이 죽을 것으로 예상됨</t>
   </si>
   <si>
@@ -63,21 +51,6 @@
   </si>
   <si>
     <t>회로 보강</t>
-  </si>
-  <si>
-    <t>+5V, +15V DC/DC output에 콘덴서 추가</t>
-  </si>
-  <si>
-    <t>15V bias Transistor에 Bias 저항 필요 여부 확인</t>
-  </si>
-  <si>
-    <t>Q1,Q2,Q3,Q4</t>
-  </si>
-  <si>
-    <t>2차측은 전류가 낮으므로 current detect이 안될것으로 판단됨 - 1차측에 연결 검토</t>
-  </si>
-  <si>
-    <t>CAS_6-NP</t>
   </si>
   <si>
     <t>Category</t>
@@ -129,18 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Check item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Current transducer의 Vout 확인 - Power별로 Vout 측정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. OP-Amp trim-R 설정치 확인 - 사용하지 않을 것으로 보임</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Load Short 발생시 2차측 전압이 역으로 유기되는지 확인 필요 - Pipette dead 원인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -256,6 +217,84 @@
   </si>
   <si>
     <t>H/W ID 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#01,#02 정상 동작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current Transducer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0A : Vout=2.5V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차측은 전류가 낮으므로 current detect이 안될것으로 판단됨 - 1차측에 연결 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OP-Amp trim-R 설정치 확인 - 사용하지 않을 것으로 보임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current transducer의 Vout 확인 - Power별로 Vout 측정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FST10-5FFM : +5V, +15V DC/DC output에 콘덴서 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1,Q2,Q3,Q4 : 15V bias Transistor에 Bias 저항 필요 여부 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fuse dead 발생 여부(250VAC 5A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC-DC Regulator(FST10-5FFM)가 dead 되는지 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불량 Board #01,#02 원인 분석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하네스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>러그 작업 불량 : 압착 불량
+ - wire가 얇은 경우, 한번 접어서 압착을 해야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FST10-5FFM를 사용하지 않고 외부 SMPS를 사용하도록 검토</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -574,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -730,9 +769,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -742,6 +778,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -751,9 +855,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -802,7 +903,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -837,7 +938,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1048,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1069,16 +1170,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E5" s="49" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G5" s="49" t="s">
         <v>4</v>
@@ -1087,7 +1188,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -1095,20 +1196,20 @@
         <v>1</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E6" s="53">
         <v>43194</v>
       </c>
       <c r="F6" s="53"/>
       <c r="G6" s="52" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H6" s="54" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I6" s="55"/>
     </row>
@@ -1420,7 +1521,7 @@
     <col min="1" max="1" width="4.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.75" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="62" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="61" customWidth="1"/>
     <col min="5" max="5" width="66.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="69.625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
@@ -1441,7 +1542,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -1452,13 +1553,13 @@
         <v>43150</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -1469,13 +1570,13 @@
         <v>43150</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -1486,13 +1587,13 @@
         <v>43150</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -1503,13 +1604,13 @@
         <v>43150</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -1520,13 +1621,13 @@
         <v>43169</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -1537,13 +1638,13 @@
         <v>43193</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -1554,13 +1655,13 @@
         <v>43193</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -1571,10 +1672,10 @@
         <v>43196</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1718,7 +1819,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="14"/>
-      <c r="D28" s="63"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="15"/>
       <c r="F28" s="16"/>
     </row>
@@ -1736,245 +1837,441 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E28"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.625" customWidth="1"/>
+    <col min="2" max="2" width="4.875" customWidth="1"/>
     <col min="3" max="3" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" style="73" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" customWidth="1"/>
+    <col min="6" max="6" width="77.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="61">
+      <c r="G2" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="65">
         <v>1</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="89" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="65"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="89" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="65"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="65"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="88" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="61"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="22" t="s">
+      <c r="G6" s="89" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="65"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="78"/>
+    </row>
+    <row r="8" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="65"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="78"/>
+    </row>
+    <row r="9" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="65"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="78"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="65"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="68"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="65">
+        <v>2</v>
+      </c>
+      <c r="C11" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="61"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="61"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="61">
-        <v>2</v>
-      </c>
-      <c r="C8" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="61"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="61"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="61"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="61">
+      <c r="D11" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="65"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="65"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="72"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="65"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="81">
         <v>3</v>
       </c>
-      <c r="C12" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="23"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="61"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="23"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="25"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="25"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="25"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="25"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="25"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="25"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="25"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="25"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="23"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="25"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="25"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="25"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="84"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="23"/>
+    </row>
+    <row r="17" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="84"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="78"/>
+    </row>
+    <row r="18" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="84"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="78"/>
+    </row>
+    <row r="19" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="82"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="78"/>
+    </row>
+    <row r="20" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="B20" s="81">
+        <v>4</v>
+      </c>
+      <c r="C20" s="79" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="74">
+        <v>43198</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="84"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="78"/>
+    </row>
+    <row r="22" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="84"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="78"/>
+    </row>
+    <row r="23" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="84"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="78"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="82"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="25"/>
       <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="74"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="25"/>
       <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="74"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="25"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23"/>
-    </row>
-    <row r="28" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="25"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="23"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="25"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="23"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="25"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="25"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="23"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="25"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="23"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="25"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="23"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="25"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="23"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="25"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="23"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="25"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="23"/>
+    </row>
+    <row r="37" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B12:B13"/>
+  <mergeCells count="8">
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="B15:B19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2009,7 +2306,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -2020,10 +2317,10 @@
         <v>43169</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -2035,10 +2332,10 @@
         <v>43193</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -2050,10 +2347,10 @@
         <v>43193</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F7" s="12"/>
     </row>
@@ -2065,10 +2362,10 @@
         <v>43193</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F8" s="12"/>
     </row>
@@ -2080,10 +2377,10 @@
         <v>43193</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F9" s="12"/>
     </row>
@@ -2095,10 +2392,10 @@
         <v>43196</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -2110,10 +2407,10 @@
         <v>43196</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="64" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>29</v>
       </c>
       <c r="F11" s="12"/>
     </row>
@@ -2264,7 +2561,7 @@
   <dimension ref="B1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2281,13 +2578,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -2295,10 +2592,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E3" s="23"/>
     </row>
@@ -2306,7 +2603,7 @@
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
       <c r="D4" s="22" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E4" s="23"/>
     </row>
@@ -2314,7 +2611,7 @@
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
       <c r="D5" s="22" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E5" s="23"/>
     </row>
@@ -2322,7 +2619,7 @@
       <c r="B6" s="31"/>
       <c r="C6" s="32"/>
       <c r="D6" s="22" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E6" s="23"/>
     </row>
@@ -2337,10 +2634,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E8" s="23"/>
     </row>

</xml_diff>